<commit_message>
fix incorrect section number
</commit_message>
<xml_diff>
--- a/data/sum/asignaturas programadas xlsx/todo-en-uno.xlsx
+++ b/data/sum/asignaturas programadas xlsx/todo-en-uno.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\sum\asignaturas programadas xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98C47D0-809E-4682-B000-2E290D7F7C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66AC1E5-BE52-460C-BF78-00AF955FEF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D60BBF6E-17AC-4730-8091-379669949CB3}"/>
   </bookViews>
@@ -2630,9 +2630,21 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D9EF12-1ACA-495A-A434-301B1E30628B}" name="Table1" displayName="Table1" ref="A1:AC726" totalsRowShown="0">
   <autoFilter ref="A1:AC726" xr:uid="{52D9EF12-1ACA-495A-A434-301B1E30628B}">
-    <filterColumn colId="27">
+    <filterColumn colId="11">
       <filters>
-        <filter val="HUARMEY"/>
+        <filter val="402-M"/>
+        <filter val="h-M"/>
+        <filter val="huarmey402-M"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="13">
+      <filters>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="28">
+      <filters>
+        <filter val="C"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2994,7 +3006,7 @@
   <dimension ref="A1:AC726"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q730" sqref="Q730:Q731"/>
+      <selection activeCell="L365" sqref="L365:L727"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30110,7 +30122,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="344" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>500</v>
       </c>
@@ -30193,7 +30205,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="345" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>505</v>
       </c>
@@ -30276,7 +30288,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="346" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>506</v>
       </c>
@@ -30350,7 +30362,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="347" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>509</v>
       </c>
@@ -30433,7 +30445,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="348" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>510</v>
       </c>
@@ -30516,7 +30528,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="349" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>513</v>
       </c>
@@ -30599,7 +30611,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="350" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>517</v>
       </c>

</xml_diff>